<commit_message>
Added: output of tasks
</commit_message>
<xml_diff>
--- a/main/Output/task_1.xlsx
+++ b/main/Output/task_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>empno</t>
   </si>
@@ -396,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -503,56 +503,64 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>7844</v>
+        <v>7839</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>7876</v>
+        <v>7844</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>7900</v>
+        <v>7876</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>7902</v>
+        <v>7900</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
+        <v>7902</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
         <v>7934</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>